<commit_message>
exp1 analysis with BHM
</commit_message>
<xml_diff>
--- a/1_Study1_Task_Target/1_2_MaterialProc/1_2_2_Exp1_materials_for_experimenters/Exp1_Survey_Participants.xlsx
+++ b/1_Study1_Task_Target/1_2_MaterialProc/1_2_2_Exp1_materials_for_experimenters/Exp1_Survey_Participants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1_Postgraduate\TaskRelevance\1_Study1_Task_Target\1_2_MaterialProc\1_2_2_Exp1_materials_for_experimenters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{9A0B4EBF-008E-4D6D-8ABB-2BBD8A3E4B32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8830487D-3303-499F-B1AA-B96D2602E806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{F03A10D7-4C19-4777-B763-293EC50CB65E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="2" xr2:uid="{F03A10D7-4C19-4777-B763-293EC50CB65E}"/>
   </bookViews>
   <sheets>
     <sheet name="Exp1_Survey_Participants" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2113" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2119" uniqueCount="239">
   <si>
     <t>编号</t>
   </si>
@@ -744,6 +744,22 @@
   </si>
   <si>
     <t>张晴</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>中途放弃实验</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>换到第二波</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>第一波截止,熊未通过好友请求</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>不做了</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -4613,13 +4629,13 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M45" sqref="M45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4648,7 +4664,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>4</v>
       </c>
@@ -4676,8 +4692,11 @@
       <c r="I2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>5</v>
       </c>
@@ -4706,7 +4725,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>6</v>
       </c>
@@ -4735,7 +4754,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>7</v>
       </c>
@@ -4764,7 +4783,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>8</v>
       </c>
@@ -4793,7 +4812,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>9</v>
       </c>
@@ -4822,7 +4841,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>10</v>
       </c>
@@ -4851,7 +4870,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>11</v>
       </c>
@@ -4880,7 +4899,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>12</v>
       </c>
@@ -4908,8 +4927,11 @@
       <c r="I10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K10" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>13</v>
       </c>
@@ -4938,7 +4960,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>14</v>
       </c>
@@ -4967,7 +4989,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>15</v>
       </c>
@@ -4996,7 +5018,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>16</v>
       </c>
@@ -5025,7 +5047,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>17</v>
       </c>
@@ -5054,7 +5076,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>18</v>
       </c>
@@ -5081,6 +5103,9 @@
       </c>
       <c r="I16" t="s">
         <v>48</v>
+      </c>
+      <c r="K16" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
@@ -5639,6 +5664,9 @@
       <c r="I35" t="s">
         <v>88</v>
       </c>
+      <c r="K35" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36">
@@ -5783,6 +5811,9 @@
       </c>
       <c r="I40" t="s">
         <v>97</v>
+      </c>
+      <c r="K40" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
@@ -7546,8 +7577,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -8022,7 +8053,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>19</v>
       </c>
@@ -8051,7 +8082,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>20</v>
       </c>
@@ -8080,7 +8111,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>21</v>
       </c>
@@ -8109,7 +8140,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>22</v>
       </c>
@@ -8138,7 +8169,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>23</v>
       </c>
@@ -8167,7 +8198,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>24</v>
       </c>
@@ -8196,7 +8227,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>25</v>
       </c>
@@ -8224,8 +8255,11 @@
       <c r="I23" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K23" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>26</v>
       </c>
@@ -8254,7 +8288,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>27</v>
       </c>
@@ -8283,7 +8317,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>28</v>
       </c>
@@ -8312,7 +8346,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>29</v>
       </c>
@@ -8341,7 +8375,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>30</v>
       </c>
@@ -8370,7 +8404,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>31</v>
       </c>
@@ -8399,7 +8433,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>33</v>
       </c>
@@ -8428,7 +8462,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>34</v>
       </c>
@@ -8457,7 +8491,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>35</v>
       </c>
@@ -9040,7 +9074,7 @@
         <v>230</v>
       </c>
       <c r="K51" t="s">
-        <v>221</v>
+        <v>237</v>
       </c>
     </row>
     <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.3">

</xml_diff>